<commit_message>
The simulations done again and Commented report
The simulations for R-L load and R-L load with line ind. have been done again. Also, some comments have been done for Part1
</commit_message>
<xml_diff>
--- a/Simulation Results_corrected_v2.xlsx
+++ b/Simulation Results_corrected_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faati\Desktop\EE463-Lab3-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryusl\OneDrive\Masaüstü\2020-21 Fall\EE463\LABS\Lab #3\EE463-Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B82DE7-732D-453B-AA51-E7E33BBF7BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5953BE7F-4B43-4A47-A90C-3AAF68D96B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF9D3880-F8E8-4D05-ACEA-EE60A48F8178}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="244">
   <si>
     <t>R Load</t>
   </si>
@@ -427,15 +427,6 @@
     <t>300V</t>
   </si>
   <si>
-    <t>3.594A</t>
-  </si>
-  <si>
-    <t>1524W</t>
-  </si>
-  <si>
-    <t>27.67VAR</t>
-  </si>
-  <si>
     <t>0.9998</t>
   </si>
   <si>
@@ -448,18 +439,6 @@
     <t>%29.51</t>
   </si>
   <si>
-    <t>4.594A</t>
-  </si>
-  <si>
-    <t>46.5V</t>
-  </si>
-  <si>
-    <t>1.766A</t>
-  </si>
-  <si>
-    <t>650.3VAR</t>
-  </si>
-  <si>
     <t>0.4965</t>
   </si>
   <si>
@@ -472,18 +451,6 @@
     <t>%29.25</t>
   </si>
   <si>
-    <t>158.9V</t>
-  </si>
-  <si>
-    <t>2.254A</t>
-  </si>
-  <si>
-    <t>358.1W</t>
-  </si>
-  <si>
-    <t>297.7V</t>
-  </si>
-  <si>
     <t>-11.05°</t>
   </si>
   <si>
@@ -493,9 +460,6 @@
     <t>1459W</t>
   </si>
   <si>
-    <t>284.9VAR</t>
-  </si>
-  <si>
     <t>0.9815</t>
   </si>
   <si>
@@ -514,9 +478,6 @@
     <t>1458W</t>
   </si>
   <si>
-    <t>57.52V</t>
-  </si>
-  <si>
     <t>-60.8°</t>
   </si>
   <si>
@@ -547,9 +508,6 @@
     <t>344.7W</t>
   </si>
   <si>
-    <t>288.8V</t>
-  </si>
-  <si>
     <t>70usec</t>
   </si>
   <si>
@@ -562,36 +520,9 @@
     <t>%30.01</t>
   </si>
   <si>
-    <t>0.866A</t>
-  </si>
-  <si>
-    <t>356.3VAR</t>
-  </si>
-  <si>
-    <t>89.58W</t>
-  </si>
-  <si>
     <t>0.2438</t>
   </si>
   <si>
-    <t>80.28V</t>
-  </si>
-  <si>
-    <t>1.111A</t>
-  </si>
-  <si>
-    <t>89.21W</t>
-  </si>
-  <si>
-    <t>322.6V</t>
-  </si>
-  <si>
-    <t>30usec</t>
-  </si>
-  <si>
-    <t>842usec</t>
-  </si>
-  <si>
     <t>284.8VAR</t>
   </si>
   <si>
@@ -670,7 +601,439 @@
     <t>182.3W</t>
   </si>
   <si>
-    <t>371.9W</t>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>3.44</t>
+  </si>
+  <si>
+    <t>464</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>28.7</t>
+  </si>
+  <si>
+    <t>27.6</t>
+  </si>
+  <si>
+    <t>323</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>4.07</t>
+  </si>
+  <si>
+    <t>1350</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>2.03</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>245</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>1.87</t>
+  </si>
+  <si>
+    <t>375</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>28.4</t>
+  </si>
+  <si>
+    <t>27.3</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>3.64</t>
+  </si>
+  <si>
+    <t>1190</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>0.44</t>
+  </si>
+  <si>
+    <t>29.9</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>476</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>2.81</t>
+  </si>
+  <si>
+    <t>348</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>18.5</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>24.3</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>3.40</t>
+  </si>
+  <si>
+    <t>1050</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>30.1</t>
+  </si>
+  <si>
+    <t>28.9</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>1.49</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>50.9</t>
+  </si>
+  <si>
+    <t>0.147</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>47.1</t>
+  </si>
+  <si>
+    <t>42.5</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>336</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>29.1</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>2.86</t>
+  </si>
+  <si>
+    <t>365</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25.1</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>3.49</t>
+  </si>
+  <si>
+    <t>1090</t>
+  </si>
+  <si>
+    <t>1.24</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>30.4</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>1.53</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>66.3</t>
+  </si>
+  <si>
+    <t>54.9</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>46.1</t>
+  </si>
+  <si>
+    <t>Experimental Results</t>
+  </si>
+  <si>
+    <t>138V</t>
+  </si>
+  <si>
+    <t>3.507A</t>
+  </si>
+  <si>
+    <t>483.8W</t>
+  </si>
+  <si>
+    <t>8.783VAR</t>
+  </si>
+  <si>
+    <t>322.7V</t>
+  </si>
+  <si>
+    <t>4.483A</t>
+  </si>
+  <si>
+    <t>1447W</t>
+  </si>
+  <si>
+    <t>45.02V</t>
+  </si>
+  <si>
+    <t>1.723A</t>
+  </si>
+  <si>
+    <t>118.1W</t>
+  </si>
+  <si>
+    <t>206.4VAR</t>
+  </si>
+  <si>
+    <t>155.1V</t>
+  </si>
+  <si>
+    <t>2.199A</t>
+  </si>
+  <si>
+    <t>341W</t>
+  </si>
+  <si>
+    <t>292.1V</t>
+  </si>
+  <si>
+    <t>130V</t>
+  </si>
+  <si>
+    <t>3.22A</t>
+  </si>
+  <si>
+    <t>80.23VAR</t>
+  </si>
+  <si>
+    <t>410.9W</t>
+  </si>
+  <si>
+    <t>297.8V</t>
+  </si>
+  <si>
+    <t>4.137A</t>
+  </si>
+  <si>
+    <t>1232W</t>
+  </si>
+  <si>
+    <t>44.37V</t>
+  </si>
+  <si>
+    <t>810usec</t>
+  </si>
+  <si>
+    <t>1.593A</t>
+  </si>
+  <si>
+    <t>101W</t>
+  </si>
+  <si>
+    <t>180.7VAR</t>
+  </si>
+  <si>
+    <t>143.3V</t>
+  </si>
+  <si>
+    <t>2.033A</t>
+  </si>
+  <si>
+    <t>291.2W</t>
+  </si>
+  <si>
+    <t>264.9V</t>
+  </si>
+  <si>
+    <t>27.21W</t>
+  </si>
+  <si>
+    <t>108.2VAR</t>
+  </si>
+  <si>
+    <t>135V</t>
+  </si>
+  <si>
+    <t>0.827A</t>
+  </si>
+  <si>
+    <t>76.63V</t>
+  </si>
+  <si>
+    <t>81.23W</t>
+  </si>
+  <si>
+    <t>1.061A</t>
+  </si>
+  <si>
+    <t>314.0V</t>
+  </si>
+  <si>
+    <t>25usec</t>
   </si>
 </sst>
 </file>
@@ -859,25 +1222,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -938,6 +1289,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -976,7 +1343,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1272,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69AF2D95-14B6-4E63-BABD-F8A5322C8551}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,825 +1658,1093 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="40" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="34" t="s">
+      <c r="D4" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" s="36" t="s">
+      <c r="H4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="27" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="30" t="s">
+      <c r="D5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="N5" s="32" t="s">
-        <v>121</v>
+      <c r="M5" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="C6" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="H6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="I6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="J6" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" s="32" t="s">
-        <v>38</v>
+      <c r="K6" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" s="18" t="s">
+      <c r="C7" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="N8" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>95</v>
+      <c r="C8" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="L9" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>82</v>
+      <c r="C9" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L10" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="N10" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>94</v>
+      <c r="C10" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="N11" s="32" t="s">
-        <v>69</v>
+      <c r="D11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="27" t="s">
+      <c r="D12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="29" t="s">
+      <c r="M12" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="37"/>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="M12" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="32" t="s">
-        <v>80</v>
+      <c r="I13" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="N13" s="27" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
-      <c r="B13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I13" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="K13" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="M13" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="N13" s="39" t="s">
-        <v>109</v>
-      </c>
+    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
     </row>
     <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="40" t="s">
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
     </row>
     <row r="17" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="N17" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="25" t="s">
+      <c r="N18" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="16"/>
+      <c r="C19" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="L19" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="M19" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" s="33" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="17"/>
+      <c r="C20" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="N20" s="33" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="17"/>
+      <c r="C21" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="N21" s="33" t="s">
+        <v>133</v>
+      </c>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="18" t="s">
+      <c r="C22" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="L22" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="O22" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="19"/>
+      <c r="C23" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="L23" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="N23" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="O23" s="7">
+        <v>720</v>
+      </c>
     </row>
     <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="44"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="19"/>
+      <c r="C24" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="L24" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="N24" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="O24" s="7">
+        <v>80</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="38"/>
+      <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="19"/>
+      <c r="C25" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="L25" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="N25" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="O25" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="26" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="17"/>
+      <c r="C26" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="L26" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="M26" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="N26" s="33" t="s">
+        <v>184</v>
+      </c>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="17"/>
+      <c r="C27" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="K27" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="L27" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="N27" s="33" t="s">
+        <v>192</v>
+      </c>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="43"/>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="37"/>
+      <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="13"/>
+      <c r="C28" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="J28" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="L28" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="28"/>
+      <c r="F33" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="A26:A28"/>
@@ -2122,6 +2757,7 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
The part 1.3.3 and 1.3.4 completed
The parts 1.3.3 and 1.3.4 have been completed and other parts are commented to change them
</commit_message>
<xml_diff>
--- a/Simulation Results_corrected_v2.xlsx
+++ b/Simulation Results_corrected_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryusl\OneDrive\Masaüstü\2020-21 Fall\EE463\LABS\Lab #3\EE463-Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5953BE7F-4B43-4A47-A90C-3AAF68D96B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A3D352-A074-4B16-B45B-7FFFF6498D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF9D3880-F8E8-4D05-ACEA-EE60A48F8178}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="246">
   <si>
     <t>R Load</t>
   </si>
@@ -397,12 +397,6 @@
     <t>141.4V</t>
   </si>
   <si>
-    <t>1527W</t>
-  </si>
-  <si>
-    <t>23.81VAR</t>
-  </si>
-  <si>
     <t>0.9999</t>
   </si>
   <si>
@@ -412,21 +406,6 @@
     <t>%29.19</t>
   </si>
   <si>
-    <t>330.7V</t>
-  </si>
-  <si>
-    <t>4.593A</t>
-  </si>
-  <si>
-    <t>1519W</t>
-  </si>
-  <si>
-    <t>46.4V</t>
-  </si>
-  <si>
-    <t>300V</t>
-  </si>
-  <si>
     <t>0.9998</t>
   </si>
   <si>
@@ -565,42 +544,9 @@
     <t>112.9W</t>
   </si>
   <si>
-    <t>3.599A</t>
-  </si>
-  <si>
     <t>-0.8936°</t>
   </si>
   <si>
-    <t>1.011A</t>
-  </si>
-  <si>
-    <t>63.6W</t>
-  </si>
-  <si>
-    <t>424VAR</t>
-  </si>
-  <si>
-    <t>0.1484</t>
-  </si>
-  <si>
-    <t>-81.47°</t>
-  </si>
-  <si>
-    <t>%104.7</t>
-  </si>
-  <si>
-    <t>%72.3</t>
-  </si>
-  <si>
-    <t>114.4V</t>
-  </si>
-  <si>
-    <t>1.594A</t>
-  </si>
-  <si>
-    <t>182.3W</t>
-  </si>
-  <si>
     <t>0.93</t>
   </si>
   <si>
@@ -1034,6 +980,66 @@
   </si>
   <si>
     <t>25usec</t>
+  </si>
+  <si>
+    <t>0.6359</t>
+  </si>
+  <si>
+    <t>-50.51</t>
+  </si>
+  <si>
+    <t>%62.8</t>
+  </si>
+  <si>
+    <t>%53.18</t>
+  </si>
+  <si>
+    <t>Simulation Results</t>
+  </si>
+  <si>
+    <t>139V</t>
+  </si>
+  <si>
+    <t>3.537A</t>
+  </si>
+  <si>
+    <t>491.6W</t>
+  </si>
+  <si>
+    <t>7.688VAR</t>
+  </si>
+  <si>
+    <t>325.1V</t>
+  </si>
+  <si>
+    <t>4.515A</t>
+  </si>
+  <si>
+    <t>1467W</t>
+  </si>
+  <si>
+    <t>45.34V</t>
+  </si>
+  <si>
+    <t>156.3V</t>
+  </si>
+  <si>
+    <t>2.173A</t>
+  </si>
+  <si>
+    <t>339.6W</t>
+  </si>
+  <si>
+    <t>292.4V</t>
+  </si>
+  <si>
+    <t>154.2W</t>
+  </si>
+  <si>
+    <t>187.1VAR</t>
+  </si>
+  <si>
+    <t>1.745A</t>
   </si>
 </sst>
 </file>
@@ -1639,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69AF2D95-14B6-4E63-BABD-F8A5322C8551}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,1106 +1664,1128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="C1" s="34" t="s">
+      <c r="A1" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="34" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N4" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="C5" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="H5" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="J5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="24" t="s">
+      <c r="K5" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="38"/>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="H7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="I7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="J7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="L5" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N5" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="J8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C9" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="F9" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="L9" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="M9" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="N9" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="M6" s="19" t="s">
+      <c r="O9" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="N7" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="N9" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="38"/>
       <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="38"/>
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="N10" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="C11" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11" s="20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="5" t="s">
-        <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="37"/>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
+      <c r="B13" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="37"/>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="M14" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="N14" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="K13" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="M13" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" s="27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="C16" s="34" t="s">
+      <c r="A16" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="C17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="34" t="s">
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
     </row>
     <row r="18" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M18" s="12" t="s">
+      <c r="M19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="13" t="s">
+      <c r="N19" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
+    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C20" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="L20" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="38"/>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="K21" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="L21" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="M21" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="23" t="s">
+      <c r="N21" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="30" t="s">
+    </row>
+    <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="J19" s="30" t="s">
+      <c r="D22" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="K19" s="31" t="s">
+      <c r="E22" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="L19" s="31" t="s">
+      <c r="F22" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="M19" s="32" t="s">
+      <c r="G22" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="N19" s="33" t="s">
+      <c r="I22" s="30" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="1" t="s">
+      <c r="J22" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38"/>
+      <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="29" t="s">
+      <c r="C23" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="L23" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="N23" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="L24" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="N24" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="O24" s="7">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="39"/>
+      <c r="B25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="L25" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="N25" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="O25" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="39"/>
+      <c r="B26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L26" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="M26" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="N26" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O26" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K27" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="L27" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="N27" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="36"/>
+      <c r="B28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="L28" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="36"/>
+      <c r="B29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="L29" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="K20" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="L20" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="M20" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N20" s="33" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="K21" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="L21" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="M21" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="N21" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="L22" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="M22" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="N22" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="K23" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="L23" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="M23" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="N23" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="O23" s="7">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="J24" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="K24" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="L24" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="M24" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="N24" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="O24" s="7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="J25" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="K25" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="L25" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="M25" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="N25" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="O25" s="7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="J26" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="K26" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="L26" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="M26" s="32" t="s">
+      <c r="M29" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="N26" s="33" t="s">
+      <c r="N29" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
-      <c r="B27" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="J27" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="K27" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="L27" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="M27" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="N27" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="H28" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="J28" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="K28" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="L28" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="M28" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="N28" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D33" s="28"/>
-      <c r="F33" s="28"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D34" s="28"/>
+      <c r="F34" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A15:N15"/>
+  <mergeCells count="14">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="A16:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>